<commit_message>
Experiments - Single weighted
Bug fixes on experiments and results procedures
</commit_message>
<xml_diff>
--- a/results/Sum_result_analysis_credibility.xlsx
+++ b/results/Sum_result_analysis_credibility.xlsx
@@ -22,8 +22,8 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
     <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="11" r:id="rId8"/>
-    <pivotCache cacheId="19" r:id="rId9"/>
+    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="11" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="32">
   <si>
     <t>method</t>
   </si>
@@ -125,6 +125,12 @@
   <si>
     <t>euro-first-2018</t>
   </si>
+  <si>
+    <t>w_all_grades</t>
+  </si>
+  <si>
+    <t>w_crowd_grades</t>
+  </si>
 </sst>
 </file>
 
@@ -178,103 +184,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
@@ -300,40 +210,40 @@
       <numFmt numFmtId="165" formatCode="0.00000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000"/>
+      <numFmt numFmtId="167" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.00000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -367,130 +277,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44171.466845138886" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Table1"/>
-  </cacheSource>
-  <cacheFields count="11">
-    <cacheField name="method" numFmtId="0">
-      <sharedItems count="11">
-        <s v="Kalai"/>
-        <s v="Nash"/>
-        <s v="crowd_majority"/>
-        <s v="crowd_mean"/>
-        <s v="crowd_median"/>
-        <s v="expert_majority"/>
-        <s v="expert_mean"/>
-        <s v="expert_median"/>
-        <s v="majority"/>
-        <s v="mean"/>
-        <s v="median"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="rel-crowd_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.96473949025896599" maxValue="1"/>
-    </cacheField>
-    <cacheField name="rel-expert_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.95325986518928896" maxValue="1"/>
-    </cacheField>
-    <cacheField name="rel-satisfaction_area" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.92526729521434004" maxValue="0.99136900292696495"/>
-    </cacheField>
-    <cacheField name="rel-satisfaction_sum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.96159125684520597" maxValue="0.99567667516185898"/>
-    </cacheField>
-    <cacheField name="avg_gain" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8.5736883252808404E-17" maxValue="2.6068282698403999E-2"/>
-    </cacheField>
-    <cacheField name="crowd_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.6479141479910098" maxValue="4.8177919479002398"/>
-    </cacheField>
-    <cacheField name="expert_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.7141532992491397" maxValue="4.9452971549505502"/>
-    </cacheField>
-    <cacheField name="satisfaction_area" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="22.048235258114101" maxValue="23.623375771724799"/>
-    </cacheField>
-    <cacheField name="satisfaction_sum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.3881011211020606" maxValue="9.7208800972354705"/>
-    </cacheField>
-    <cacheField name="expert_type" numFmtId="0">
-      <sharedItems count="1">
-        <s v="journal"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44171.466905092595" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Table13"/>
-  </cacheSource>
-  <cacheFields count="11">
-    <cacheField name="method" numFmtId="0">
-      <sharedItems count="11">
-        <s v="Kalai"/>
-        <s v="Nash"/>
-        <s v="crowd_majority"/>
-        <s v="crowd_mean"/>
-        <s v="crowd_median"/>
-        <s v="expert_majority"/>
-        <s v="expert_mean"/>
-        <s v="expert_median"/>
-        <s v="majority"/>
-        <s v="mean"/>
-        <s v="median"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="rel-crowd_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.93748602839737105" maxValue="1"/>
-    </cacheField>
-    <cacheField name="rel-expert_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.87694661982621003" maxValue="1"/>
-    </cacheField>
-    <cacheField name="rel-satisfaction_area" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.859362946887402" maxValue="0.96194260005420096"/>
-    </cacheField>
-    <cacheField name="rel-satisfaction_sum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.926068664165141" maxValue="0.98114657653109305"/>
-    </cacheField>
-    <cacheField name="avg_gain" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8.5197940036970901E-17" maxValue="0.109507332018559"/>
-    </cacheField>
-    <cacheField name="crowd_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.3861067434146799" maxValue="4.6785835847737696"/>
-    </cacheField>
-    <cacheField name="expert_sat" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.3203129144174799" maxValue="4.9265403580364397"/>
-    </cacheField>
-    <cacheField name="satisfaction_area" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="19.807513874707801" maxValue="22.171879141704"/>
-    </cacheField>
-    <cacheField name="satisfaction_sum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8.8950042988588809" maxValue="9.4240344736450901"/>
-    </cacheField>
-    <cacheField name="expert_type" numFmtId="0">
-      <sharedItems count="1">
-        <s v="science"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44173.927070254627" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
   <cacheSource type="worksheet">
     <worksheetSource name="Table134"/>
@@ -552,7 +338,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44173.93110509259" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="11">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1345"/>
@@ -614,303 +400,135 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="11">
-  <r>
-    <x v="0"/>
-    <n v="0.99291615475318895"/>
-    <n v="0.99795852659135598"/>
-    <n v="0.99091917507803795"/>
-    <n v="0.99547026717014997"/>
-    <n v="8.5736883252808404E-17"/>
-    <n v="4.7836634553099797"/>
-    <n v="4.9352014623108902"/>
-    <n v="23.612656804038199"/>
-    <n v="9.7188649176208894"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="0.99422703749458596"/>
-    <n v="0.997088936642196"/>
-    <n v="0.99136900292696495"/>
-    <n v="0.99567667516185898"/>
-    <n v="4.5813888621856497E-3"/>
-    <n v="4.7899790156261401"/>
-    <n v="4.9309010816093304"/>
-    <n v="23.623375771724799"/>
-    <n v="9.7208800972354705"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="0.97211803579877398"/>
-    <n v="0.95325986518928896"/>
-    <n v="0.92712783124393205"/>
-    <n v="0.96256580735138397"/>
-    <n v="2.6068282698403999E-2"/>
-    <n v="4.6834624452799201"/>
-    <n v="4.7141532992491397"/>
-    <n v="22.092570053366"/>
-    <n v="9.3976157445291104"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="0.99877715067487205"/>
-    <n v="0.97636044288251"/>
-    <n v="0.97532377895089495"/>
-    <n v="0.98742241652248697"/>
-    <n v="2.2502491239377899E-2"/>
-    <n v="4.8119005142681601"/>
-    <n v="4.8283925203931402"/>
-    <n v="23.241033420683799"/>
-    <n v="9.6402930346613207"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="1"/>
-    <n v="0.979893044890639"/>
-    <n v="0.98003302565105799"/>
-    <n v="0.98981522478699802"/>
-    <n v="2.01377419974587E-2"/>
-    <n v="4.8177919479002398"/>
-    <n v="4.8458622870535297"/>
-    <n v="23.3532502683674"/>
-    <n v="9.6636542349537802"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="0.96473949025896599"/>
-    <n v="0.95852419472220696"/>
-    <n v="0.92526729521434004"/>
-    <n v="0.96159125684520597"/>
-    <n v="2.0552383596122301E-2"/>
-    <n v="4.6479141479910098"/>
-    <n v="4.74018697311101"/>
-    <n v="22.048235258114101"/>
-    <n v="9.3881011211020606"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="0.98937983137962204"/>
-    <n v="0.997728830993861"/>
-    <n v="0.98722503343323798"/>
-    <n v="0.99360884983925302"/>
-    <n v="9.9207785631803304E-3"/>
-    <n v="4.7666261850356504"/>
-    <n v="4.9340655493260801"/>
-    <n v="23.524628939568501"/>
-    <n v="9.7006917343617598"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="0.98863885747036995"/>
-    <n v="1"/>
-    <n v="0.98867895140215201"/>
-    <n v="0.99439361656729996"/>
-    <n v="1.14555245953632E-2"/>
-    <n v="4.7630563269020598"/>
-    <n v="4.9452971549505502"/>
-    <n v="23.559274415087302"/>
-    <n v="9.7083534818525905"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="0.97211518792007501"/>
-    <n v="0.95340048107803799"/>
-    <n v="0.92725626760020197"/>
-    <n v="0.96263562816939796"/>
-    <n v="2.6002825520783202E-2"/>
-    <n v="4.6834487247928598"/>
-    <n v="4.7148486866037196"/>
-    <n v="22.095630568974201"/>
-    <n v="9.3982974113966105"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <n v="0.99881475717850599"/>
-    <n v="0.97673379272133198"/>
-    <n v="0.97573105038694496"/>
-    <n v="0.98763008708502698"/>
-    <n v="2.21694835358664E-2"/>
-    <n v="4.8120816945785396"/>
-    <n v="4.8302388462888697"/>
-    <n v="23.250738309727701"/>
-    <n v="9.6423205408674502"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="0.99999612362672496"/>
-    <n v="0.98039854755280498"/>
-    <n v="0.98053183840200098"/>
-    <n v="0.99006936415732905"/>
-    <n v="1.96274434065591E-2"/>
-    <n v="4.8177732723402897"/>
-    <n v="4.8483621479305503"/>
-    <n v="23.365136499448301"/>
-    <n v="9.6661354202708605"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44185.885681481479" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="method" numFmtId="0">
+      <sharedItems count="13">
+        <s v="Kalai"/>
+        <s v="Nash"/>
+        <s v="crowd_majority"/>
+        <s v="crowd_mean"/>
+        <s v="crowd_median"/>
+        <s v="expert_majority"/>
+        <s v="expert_mean"/>
+        <s v="expert_median"/>
+        <s v="majority"/>
+        <s v="mean"/>
+        <s v="median"/>
+        <s v="w_all_grades"/>
+        <s v="w_crowd_grades"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="rel-crowd_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.96473949025896599" maxValue="1"/>
+    </cacheField>
+    <cacheField name="rel-expert_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.95325986518928896" maxValue="1"/>
+    </cacheField>
+    <cacheField name="rel-satisfaction_area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.92526729521434004" maxValue="0.99136899635387199"/>
+    </cacheField>
+    <cacheField name="rel-satisfaction_sum" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.96159125684520597" maxValue="0.99567667094747503"/>
+    </cacheField>
+    <cacheField name="avg_gain" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8.82519515933832E-17" maxValue="2.6068282698403999E-2"/>
+    </cacheField>
+    <cacheField name="crowd_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.6479141479910098" maxValue="4.8177919479002398"/>
+    </cacheField>
+    <cacheField name="expert_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.7141532992491397" maxValue="4.9452971549505502"/>
+    </cacheField>
+    <cacheField name="satisfaction_area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="22.048235258114101" maxValue="23.623375615094201"/>
+    </cacheField>
+    <cacheField name="satisfaction_sum" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.3881011211020606" maxValue="9.7208800560900901"/>
+    </cacheField>
+    <cacheField name="expert_type" numFmtId="0">
+      <sharedItems count="1">
+        <s v="journal"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="11">
-  <r>
-    <x v="0"/>
-    <n v="0.96190349137870201"/>
-    <n v="0.99582921606728303"/>
-    <n v="0.95773497922703299"/>
-    <n v="0.97930425089508899"/>
-    <n v="8.5197940036970901E-17"/>
-    <n v="4.5003458849009599"/>
-    <n v="4.9059928226672698"/>
-    <n v="22.074897408647601"/>
-    <n v="9.4063387075682297"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="0.96962621592908704"/>
-    <n v="0.99208710803720401"/>
-    <n v="0.96194260005420096"/>
-    <n v="0.98114657653109305"/>
-    <n v="3.1134989869910399E-2"/>
-    <n v="4.5364772972121097"/>
-    <n v="4.8875571764329599"/>
-    <n v="22.171879141704"/>
-    <n v="9.4240344736450901"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="0.97779409121374306"/>
-    <n v="0.87694661982621003"/>
-    <n v="0.859362946887402"/>
-    <n v="0.926068664165141"/>
-    <n v="0.10542656968555"/>
-    <n v="4.5746913844414099"/>
-    <n v="4.3203129144174799"/>
-    <n v="19.807513874707801"/>
-    <n v="8.8950042988588809"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="0.99670467529967799"/>
-    <n v="0.91591292499762"/>
-    <n v="0.91386219548071701"/>
-    <n v="0.95526597853435102"/>
-    <n v="8.0658901705544905E-2"/>
-    <n v="4.6631661327243403"/>
-    <n v="4.5122819894479802"/>
-    <n v="21.063670690152598"/>
-    <n v="9.1754481221723196"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="1"/>
-    <n v="0.89033862681064602"/>
-    <n v="0.89169042196672099"/>
-    <n v="0.94375385638417997"/>
-    <n v="0.109507332018559"/>
-    <n v="4.6785835847737696"/>
-    <n v="4.3862891773013901"/>
-    <n v="20.552632003767499"/>
-    <n v="9.0648727620751597"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="0.93748602839737105"/>
-    <n v="0.95982525786682305"/>
-    <n v="0.90042598168243204"/>
-    <n v="0.94894398731637797"/>
-    <n v="4.5231716332018397E-2"/>
-    <n v="4.3861067434146799"/>
-    <n v="4.7286178695436503"/>
-    <n v="20.753978502239399"/>
-    <n v="9.1147246129583301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="0.95501058898561197"/>
-    <n v="0.99773374242231705"/>
-    <n v="0.95288804244967495"/>
-    <n v="0.97692361591599997"/>
-    <n v="4.3222117792861003E-2"/>
-    <n v="4.46809686491319"/>
-    <n v="4.9153755486182797"/>
-    <n v="21.963180039618599"/>
-    <n v="9.3834724135315497"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="0.95259848705990202"/>
-    <n v="1"/>
-    <n v="0.95260358085937102"/>
-    <n v="0.97691107978872205"/>
-    <n v="4.7759946116156402E-2"/>
-    <n v="4.4568116444387798"/>
-    <n v="4.9265403580364397"/>
-    <n v="21.956623465452601"/>
-    <n v="9.3833520024752204"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <n v="0.97804207187291303"/>
-    <n v="0.877823373948869"/>
-    <n v="0.86040708496741203"/>
-    <n v="0.92663914746585796"/>
-    <n v="0.104903012261753"/>
-    <n v="4.5758515826827404"/>
-    <n v="4.3246322789868303"/>
-    <n v="19.8315802829487"/>
-    <n v="8.9004838616695707"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <n v="0.99650135139021201"/>
-    <n v="0.91717017533001899"/>
-    <n v="0.91492138156367198"/>
-    <n v="0.95581179414576001"/>
-    <n v="7.9197571790708396E-2"/>
-    <n v="4.6622148648191102"/>
-    <n v="4.5184758839507104"/>
-    <n v="21.088083940816901"/>
-    <n v="9.1806907487698304"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <n v="0.99999231369169395"/>
-    <n v="0.89134403879117297"/>
-    <n v="0.89268299298064202"/>
-    <n v="0.94426579581275305"/>
-    <n v="0.108495591544937"/>
-    <n v="4.6785476237378996"/>
-    <n v="4.3912423799999196"/>
-    <n v="20.575509839262899"/>
-    <n v="9.0697900037378503"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ana Kovačević" refreshedDate="44185.887674074074" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table13"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="method" numFmtId="0">
+      <sharedItems count="13">
+        <s v="Kalai"/>
+        <s v="Nash"/>
+        <s v="crowd_majority"/>
+        <s v="crowd_mean"/>
+        <s v="crowd_median"/>
+        <s v="expert_majority"/>
+        <s v="expert_mean"/>
+        <s v="expert_median"/>
+        <s v="majority"/>
+        <s v="mean"/>
+        <s v="median"/>
+        <s v="w_all_grades"/>
+        <s v="w_crowd_grades"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="rel-crowd_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.95901469088041702" maxValue="1"/>
+    </cacheField>
+    <cacheField name="rel-expert_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.92301054765560797" maxValue="1"/>
+    </cacheField>
+    <cacheField name="rel-satisfaction_area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.90318756362812402" maxValue="0.97612421834477203"/>
+    </cacheField>
+    <cacheField name="rel-satisfaction_sum" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.94962985368997099" maxValue="0.98805621063665705"/>
+    </cacheField>
+    <cacheField name="avg_gain" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.4241887723332303E-10" maxValue="5.97486322518632E-2"/>
+    </cacheField>
+    <cacheField name="crowd_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.4868303903099997" maxValue="4.6785835847737696"/>
+    </cacheField>
+    <cacheField name="expert_sat" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.5690122845508698" maxValue="4.9501192550354798"/>
+    </cacheField>
+    <cacheField name="satisfaction_area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="20.917706722133399" maxValue="22.60691017676"/>
+    </cacheField>
+    <cacheField name="satisfaction_sum" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.1437036689922699" maxValue="9.5136996412483406"/>
+    </cacheField>
+    <cacheField name="expert_type" numFmtId="0">
+      <sharedItems count="1">
+        <s v="science"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="11">
   <r>
     <x v="0"/>
@@ -1058,7 +676,7 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="11">
   <r>
     <x v="0"/>
@@ -1206,9 +824,357 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="13">
+  <r>
+    <x v="0"/>
+    <n v="0.99291835361538405"/>
+    <n v="0.99796330261459298"/>
+    <n v="0.99092615927959304"/>
+    <n v="0.99547377144162996"/>
+    <n v="8.82519515933832E-17"/>
+    <n v="4.7836740489705596"/>
+    <n v="4.9352250811650302"/>
+    <n v="23.612823230885699"/>
+    <n v="9.7188991301355792"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0.99422706182025999"/>
+    <n v="0.997088904623606"/>
+    <n v="0.99136899635387199"/>
+    <n v="0.99567667094747503"/>
+    <n v="4.5813906131894396E-3"/>
+    <n v="4.7899791328221699"/>
+    <n v="4.9309009232678997"/>
+    <n v="23.623375615094201"/>
+    <n v="9.7208800560900901"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.97211803579877398"/>
+    <n v="0.95325986518928896"/>
+    <n v="0.92712783124393205"/>
+    <n v="0.96256580735138397"/>
+    <n v="2.6068282698403999E-2"/>
+    <n v="4.6834624452799201"/>
+    <n v="4.7141532992491397"/>
+    <n v="22.092570053366"/>
+    <n v="9.3976157445291104"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0.99877715067487205"/>
+    <n v="0.97636044288251"/>
+    <n v="0.97532377895089495"/>
+    <n v="0.98742241652248697"/>
+    <n v="2.2502491239377899E-2"/>
+    <n v="4.8119005142681601"/>
+    <n v="4.8283925203931402"/>
+    <n v="23.241033420683799"/>
+    <n v="9.6402930346613207"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="0.979893044890639"/>
+    <n v="0.98003302565105799"/>
+    <n v="0.98981522478699802"/>
+    <n v="2.01377419974587E-2"/>
+    <n v="4.8177919479002398"/>
+    <n v="4.8458622870535297"/>
+    <n v="23.3532502683674"/>
+    <n v="9.6636542349537802"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.96473949025896599"/>
+    <n v="0.95852419472220696"/>
+    <n v="0.92526729521434004"/>
+    <n v="0.96159125684520597"/>
+    <n v="2.0552383596122398E-2"/>
+    <n v="4.6479141479910098"/>
+    <n v="4.74018697311101"/>
+    <n v="22.048235258114101"/>
+    <n v="9.3881011211020606"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.98937983137962204"/>
+    <n v="0.997728830993861"/>
+    <n v="0.98722503343323798"/>
+    <n v="0.99360884983925302"/>
+    <n v="9.9207785631803408E-3"/>
+    <n v="4.7666261850356504"/>
+    <n v="4.9340655493260801"/>
+    <n v="23.524628939568501"/>
+    <n v="9.7006917343617598"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.98863885747036995"/>
+    <n v="1"/>
+    <n v="0.98867895140215201"/>
+    <n v="0.99439361656729996"/>
+    <n v="1.14555245953632E-2"/>
+    <n v="4.7630563269020598"/>
+    <n v="4.9452971549505502"/>
+    <n v="23.559274415087302"/>
+    <n v="9.7083534818525905"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.97211518792007501"/>
+    <n v="0.95340048107803799"/>
+    <n v="0.92725626760020197"/>
+    <n v="0.96263562816939796"/>
+    <n v="2.6002825520783202E-2"/>
+    <n v="4.6834487247928598"/>
+    <n v="4.7148486866037196"/>
+    <n v="22.095630568974201"/>
+    <n v="9.3982974113966105"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.99881475717850599"/>
+    <n v="0.97673379272133098"/>
+    <n v="0.97573105038694496"/>
+    <n v="0.98763008708502698"/>
+    <n v="2.21694835358664E-2"/>
+    <n v="4.8120816945785396"/>
+    <n v="4.8302388462888697"/>
+    <n v="23.250738309727701"/>
+    <n v="9.6423205408674502"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="0.99999612362672496"/>
+    <n v="0.98039854755280498"/>
+    <n v="0.98053183840200098"/>
+    <n v="0.99006936415732905"/>
+    <n v="1.96274434065591E-2"/>
+    <n v="4.8177732723402897"/>
+    <n v="4.8483621479305503"/>
+    <n v="23.365136499448301"/>
+    <n v="9.6661354202708605"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="0.998814090920082"/>
+    <n v="0.97761975181737804"/>
+    <n v="0.97662121512356104"/>
+    <n v="0.98807852313395395"/>
+    <n v="2.1308152441336499E-2"/>
+    <n v="4.8120784846840898"/>
+    <n v="4.8346201772859603"/>
+    <n v="23.2719500845661"/>
+    <n v="9.6466986619700297"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.99877816416487697"/>
+    <n v="0.97717824962597699"/>
+    <n v="0.97614797485860205"/>
+    <n v="0.987837160268353"/>
+    <n v="2.1711299529722599E-2"/>
+    <n v="4.8119053970521302"/>
+    <n v="4.8324368177549202"/>
+    <n v="23.260673221383499"/>
+    <n v="9.6443422148070201"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="13">
+  <r>
+    <x v="0"/>
+    <n v="0.97765519853992"/>
+    <n v="0.99748267749133102"/>
+    <n v="0.97524219908462595"/>
+    <n v="0.98784851190404299"/>
+    <n v="3.4241887723332303E-10"/>
+    <n v="4.5740415634576097"/>
+    <n v="4.93765820841418"/>
+    <n v="22.586482725198401"/>
+    <n v="9.5116997718717897"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0.98274182350946504"/>
+    <n v="0.99307908040916204"/>
+    <n v="0.97612421834477203"/>
+    <n v="0.98805621063665705"/>
+    <n v="1.4231195644233601E-2"/>
+    <n v="4.5978397635420203"/>
+    <n v="4.91585987770633"/>
+    <n v="22.60691017676"/>
+    <n v="9.5136996412483406"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.97779409121374306"/>
+    <n v="0.92301054765560797"/>
+    <n v="0.90318756362812402"/>
+    <n v="0.94962985368997099"/>
+    <n v="5.97486322518632E-2"/>
+    <n v="4.5746913844414099"/>
+    <n v="4.5690122845508698"/>
+    <n v="20.917706722133399"/>
+    <n v="9.1437036689922699"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="0.99670467529967799"/>
+    <n v="0.95110802073391498"/>
+    <n v="0.94789792272638795"/>
+    <n v="0.97326342038858005"/>
+    <n v="4.6260289344101597E-2"/>
+    <n v="4.6631661327243403"/>
+    <n v="4.7080981270536402"/>
+    <n v="21.953192834566"/>
+    <n v="9.3712642597779592"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="0.944000338299258"/>
+    <n v="0.94416856976965102"/>
+    <n v="0.97121055574441095"/>
+    <n v="5.60143006007644E-2"/>
+    <n v="4.6785835847737696"/>
+    <n v="4.67291425137517"/>
+    <n v="21.8668215042313"/>
+    <n v="9.35149783614896"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="0.95901469088041702"/>
+    <n v="0.95838637067937404"/>
+    <n v="0.91943391250694795"/>
+    <n v="0.95869167126113297"/>
+    <n v="3.5632998459510103E-2"/>
+    <n v="4.4868303903099997"/>
+    <n v="4.74412682726354"/>
+    <n v="21.2939700530716"/>
+    <n v="9.2309572175735592"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="0.97322972640178496"/>
+    <n v="0.99824132605718996"/>
+    <n v="0.971580206412332"/>
+    <n v="0.986088197902387"/>
+    <n v="2.5415490845142299E-2"/>
+    <n v="4.5533366221572802"/>
+    <n v="4.9414136092878502"/>
+    <n v="22.501671450306599"/>
+    <n v="9.4947502314451206"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="0.97184506146743599"/>
+    <n v="1"/>
+    <n v="0.97189913968408503"/>
+    <n v="0.98631952450498706"/>
+    <n v="2.7982666156550699E-2"/>
+    <n v="4.5468583515249996"/>
+    <n v="4.9501192550354798"/>
+    <n v="22.509057903476702"/>
+    <n v="9.4969776065605096"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="0.97781582987516502"/>
+    <n v="0.92319611447642302"/>
+    <n v="0.90338448556020401"/>
+    <n v="0.94973581646131"/>
+    <n v="5.9628081380639401E-2"/>
+    <n v="4.5747930905858896"/>
+    <n v="4.5699308624436803"/>
+    <n v="20.922267408515999"/>
+    <n v="9.1447239530295708"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="0.99669855590412104"/>
+    <n v="0.95182993538673299"/>
+    <n v="0.94861318128531202"/>
+    <n v="0.97363158353358303"/>
+    <n v="4.5535835314306501E-2"/>
+    <n v="4.6631375026207396"/>
+    <n v="4.7116716906770497"/>
+    <n v="21.969758129936"/>
+    <n v="9.3748091932977804"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="0.999993307635895"/>
+    <n v="0.94488353053645002"/>
+    <n v="0.94503982601356196"/>
+    <n v="0.97166135334265402"/>
+    <n v="5.5124972763770201E-2"/>
+    <n v="4.67855227398893"/>
+    <n v="4.6772861582744003"/>
+    <n v="21.8869996857341"/>
+    <n v="9.3558384322633206"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="0.99555757929425504"/>
+    <n v="0.95191862357264001"/>
+    <n v="0.94762096601494195"/>
+    <n v="0.97312277799432401"/>
+    <n v="4.4509003438409002E-2"/>
+    <n v="4.6577993481832101"/>
+    <n v="4.7121107077737898"/>
+    <n v="21.946778553083298"/>
+    <n v="9.3699100559570194"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="0.99555172408908998"/>
+    <n v="0.95103652609863898"/>
+    <n v="0.946736047670521"/>
+    <n v="0.97266644635435695"/>
+    <n v="4.5365352719056701E-2"/>
+    <n v="4.6577719541164297"/>
+    <n v="4.7077442200829402"/>
+    <n v="21.926283959106399"/>
+    <n v="9.3655161741993407"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G18:J30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G21:J33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
       <items count="11">
@@ -1311,7 +1277,7 @@
     <dataField name="avg_satisfaction_area" fld="8" baseField="0" baseItem="8"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="39">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1319,7 +1285,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1327,7 +1293,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1335,7 +1301,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1343,7 +1309,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1351,7 +1317,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1362,7 +1328,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1373,7 +1339,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1386,7 +1352,7 @@
     </format>
   </formats>
   <conditionalFormats count="4">
-    <conditionalFormat priority="4">
+    <conditionalFormat priority="7">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1413,7 +1379,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="6">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1440,7 +1406,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="5">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1467,7 +1433,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="4">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1505,7 +1471,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G3:J15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
@@ -1609,27 +1575,27 @@
     <dataField name="avg_satisfaction_area" fld="8" baseField="0" baseItem="9"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="46">
+    <format dxfId="13">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="4">
-    <conditionalFormat priority="8">
+    <conditionalFormat priority="11">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1640,7 +1606,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="7">
+    <conditionalFormat priority="10">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1651,7 +1617,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="6">
+    <conditionalFormat priority="9">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1662,7 +1628,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="5">
+    <conditionalFormat priority="8">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1684,11 +1650,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B3:E15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B3:E17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="12">
+      <items count="14">
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
@@ -1700,6 +1666,8 @@
         <item x="9"/>
         <item x="10"/>
         <item x="1"/>
+        <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -1731,7 +1699,7 @@
     <field x="10"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="14">
     <i>
       <x/>
     </i>
@@ -1752,6 +1720,12 @@
     </i>
     <i r="1">
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
     </i>
     <i r="1">
       <x v="8"/>
@@ -1789,27 +1763,27 @@
     <dataField name="avg_satisfaction_area" fld="8" baseField="0" baseItem="2"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="40">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="18">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="4">
-    <conditionalFormat priority="19">
+    <conditionalFormat priority="22">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1820,7 +1794,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="17">
+    <conditionalFormat priority="20">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1831,7 +1805,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="16">
+    <conditionalFormat priority="19">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1842,7 +1816,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="15">
+    <conditionalFormat priority="18">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
@@ -1864,11 +1838,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B18:E30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B21:E35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="11">
+      <items count="13">
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
@@ -1880,6 +1854,8 @@
         <item x="9"/>
         <item x="10"/>
         <item x="1"/>
+        <item x="11"/>
+        <item x="12"/>
       </items>
       <autoSortScope>
         <pivotArea dataOnly="0" outline="0" fieldPosition="0">
@@ -1910,7 +1886,7 @@
     <field x="10"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="14">
     <i>
       <x/>
     </i>
@@ -1921,10 +1897,10 @@
       <x v="6"/>
     </i>
     <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
       <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="8"/>
@@ -1933,13 +1909,19 @@
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="3"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
     </i>
     <i r="1">
       <x v="9"/>
     </i>
     <i r="1">
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
     </i>
     <i r="1">
       <x v="7"/>
@@ -1968,7 +1950,7 @@
     <dataField name="avg_satisfaction_area" fld="8" baseField="0" baseItem="5"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="57">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1976,7 +1958,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="24">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1984,7 +1966,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1992,7 +1974,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -2000,7 +1982,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -2008,7 +1990,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -2017,8 +1999,95 @@
       </pivotArea>
     </format>
   </formats>
-  <conditionalFormats count="3">
-    <conditionalFormat priority="10">
+  <conditionalFormats count="6">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="0" count="13">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="10" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="0" count="13">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="10" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="13">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="10" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="13">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -2045,7 +2114,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="11">
+    <conditionalFormat priority="14">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -2072,7 +2141,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="13">
+    <conditionalFormat priority="16">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -2110,8 +2179,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K12" totalsRowShown="0">
-  <autoFilter ref="A1:K12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K14" totalsRowShown="0">
+  <autoFilter ref="A1:K14"/>
   <tableColumns count="11">
     <tableColumn id="1" name="method"/>
     <tableColumn id="2" name="rel-crowd_sat"/>
@@ -2130,8 +2199,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:K12" totalsRowShown="0">
-  <autoFilter ref="A1:K12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:K14" totalsRowShown="0">
+  <autoFilter ref="A1:K14"/>
   <tableColumns count="11">
     <tableColumn id="1" name="method"/>
     <tableColumn id="2" name="rel-crowd_sat"/>
@@ -2452,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2512,31 +2581,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.99291615475318895</v>
+        <v>0.99291835361538405</v>
       </c>
       <c r="C2">
-        <v>0.99795852659135598</v>
+        <v>0.99796330261459298</v>
       </c>
       <c r="D2">
-        <v>0.99091917507803795</v>
+        <v>0.99092615927959304</v>
       </c>
       <c r="E2">
-        <v>0.99547026717014997</v>
+        <v>0.99547377144162996</v>
       </c>
       <c r="F2" s="1">
-        <v>8.5736883252808404E-17</v>
+        <v>8.82519515933832E-17</v>
       </c>
       <c r="G2">
-        <v>4.7836634553099797</v>
+        <v>4.7836740489705596</v>
       </c>
       <c r="H2">
-        <v>4.9352014623108902</v>
+        <v>4.9352250811650302</v>
       </c>
       <c r="I2">
-        <v>23.612656804038199</v>
+        <v>23.612823230885699</v>
       </c>
       <c r="J2">
-        <v>9.7188649176208894</v>
+        <v>9.7188991301355792</v>
       </c>
       <c r="K2" t="s">
         <v>26</v>
@@ -2547,31 +2616,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.99422703749458596</v>
+        <v>0.99422706182025999</v>
       </c>
       <c r="C3">
-        <v>0.997088936642196</v>
+        <v>0.997088904623606</v>
       </c>
       <c r="D3">
-        <v>0.99136900292696495</v>
+        <v>0.99136899635387199</v>
       </c>
       <c r="E3">
-        <v>0.99567667516185898</v>
+        <v>0.99567667094747503</v>
       </c>
       <c r="F3">
-        <v>4.5813888621856497E-3</v>
+        <v>4.5813906131894396E-3</v>
       </c>
       <c r="G3">
-        <v>4.7899790156261401</v>
+        <v>4.7899791328221699</v>
       </c>
       <c r="H3">
-        <v>4.9309010816093304</v>
+        <v>4.9309009232678997</v>
       </c>
       <c r="I3">
-        <v>23.623375771724799</v>
+        <v>23.623375615094201</v>
       </c>
       <c r="J3">
-        <v>9.7208800972354705</v>
+        <v>9.7208800560900901</v>
       </c>
       <c r="K3" t="s">
         <v>26</v>
@@ -2699,7 +2768,7 @@
         <v>0.96159125684520597</v>
       </c>
       <c r="F7">
-        <v>2.0552383596122301E-2</v>
+        <v>2.0552383596122398E-2</v>
       </c>
       <c r="G7">
         <v>4.6479141479910098</v>
@@ -2734,7 +2803,7 @@
         <v>0.99360884983925302</v>
       </c>
       <c r="F8">
-        <v>9.9207785631803304E-3</v>
+        <v>9.9207785631803408E-3</v>
       </c>
       <c r="G8">
         <v>4.7666261850356504</v>
@@ -2830,7 +2899,7 @@
         <v>0.99881475717850599</v>
       </c>
       <c r="C11">
-        <v>0.97673379272133198</v>
+        <v>0.97673379272133098</v>
       </c>
       <c r="D11">
         <v>0.97573105038694496</v>
@@ -2889,6 +2958,76 @@
         <v>9.6661354202708605</v>
       </c>
       <c r="K12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>0.998814090920082</v>
+      </c>
+      <c r="C13">
+        <v>0.97761975181737804</v>
+      </c>
+      <c r="D13">
+        <v>0.97662121512356104</v>
+      </c>
+      <c r="E13">
+        <v>0.98807852313395395</v>
+      </c>
+      <c r="F13">
+        <v>2.1308152441336499E-2</v>
+      </c>
+      <c r="G13">
+        <v>4.8120784846840898</v>
+      </c>
+      <c r="H13">
+        <v>4.8346201772859603</v>
+      </c>
+      <c r="I13">
+        <v>23.2719500845661</v>
+      </c>
+      <c r="J13">
+        <v>9.6466986619700297</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>0.99877816416487697</v>
+      </c>
+      <c r="C14">
+        <v>0.97717824962597699</v>
+      </c>
+      <c r="D14">
+        <v>0.97614797485860205</v>
+      </c>
+      <c r="E14">
+        <v>0.987837160268353</v>
+      </c>
+      <c r="F14">
+        <v>2.1711299529722599E-2</v>
+      </c>
+      <c r="G14">
+        <v>4.8119053970521302</v>
+      </c>
+      <c r="H14">
+        <v>4.8324368177549202</v>
+      </c>
+      <c r="I14">
+        <v>23.260673221383499</v>
+      </c>
+      <c r="J14">
+        <v>9.6443422148070201</v>
+      </c>
+      <c r="K14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2902,10 +3041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2962,31 +3101,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.96190349137870201</v>
+        <v>0.97765519853992</v>
       </c>
       <c r="C2">
-        <v>0.99582921606728303</v>
+        <v>0.99748267749133102</v>
       </c>
       <c r="D2">
-        <v>0.95773497922703299</v>
+        <v>0.97524219908462595</v>
       </c>
       <c r="E2">
-        <v>0.97930425089508899</v>
+        <v>0.98784851190404299</v>
       </c>
       <c r="F2" s="1">
-        <v>8.5197940036970901E-17</v>
+        <v>3.4241887723332303E-10</v>
       </c>
       <c r="G2">
-        <v>4.5003458849009599</v>
+        <v>4.5740415634576097</v>
       </c>
       <c r="H2">
-        <v>4.9059928226672698</v>
+        <v>4.93765820841418</v>
       </c>
       <c r="I2">
-        <v>22.074897408647601</v>
+        <v>22.586482725198401</v>
       </c>
       <c r="J2">
-        <v>9.4063387075682297</v>
+        <v>9.5116997718717897</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -2997,31 +3136,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.96962621592908704</v>
+        <v>0.98274182350946504</v>
       </c>
       <c r="C3">
-        <v>0.99208710803720401</v>
+        <v>0.99307908040916204</v>
       </c>
       <c r="D3">
-        <v>0.96194260005420096</v>
+        <v>0.97612421834477203</v>
       </c>
       <c r="E3">
-        <v>0.98114657653109305</v>
+        <v>0.98805621063665705</v>
       </c>
       <c r="F3">
-        <v>3.1134989869910399E-2</v>
+        <v>1.4231195644233601E-2</v>
       </c>
       <c r="G3">
-        <v>4.5364772972121097</v>
+        <v>4.5978397635420203</v>
       </c>
       <c r="H3">
-        <v>4.8875571764329599</v>
+        <v>4.91585987770633</v>
       </c>
       <c r="I3">
-        <v>22.171879141704</v>
+        <v>22.60691017676</v>
       </c>
       <c r="J3">
-        <v>9.4240344736450901</v>
+        <v>9.5136996412483406</v>
       </c>
       <c r="K3" t="s">
         <v>27</v>
@@ -3035,28 +3174,28 @@
         <v>0.97779409121374306</v>
       </c>
       <c r="C4">
-        <v>0.87694661982621003</v>
+        <v>0.92301054765560797</v>
       </c>
       <c r="D4">
-        <v>0.859362946887402</v>
+        <v>0.90318756362812402</v>
       </c>
       <c r="E4">
-        <v>0.926068664165141</v>
+        <v>0.94962985368997099</v>
       </c>
       <c r="F4">
-        <v>0.10542656968555</v>
+        <v>5.97486322518632E-2</v>
       </c>
       <c r="G4">
         <v>4.5746913844414099</v>
       </c>
       <c r="H4">
-        <v>4.3203129144174799</v>
+        <v>4.5690122845508698</v>
       </c>
       <c r="I4">
-        <v>19.807513874707801</v>
+        <v>20.917706722133399</v>
       </c>
       <c r="J4">
-        <v>8.8950042988588809</v>
+        <v>9.1437036689922699</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -3070,28 +3209,28 @@
         <v>0.99670467529967799</v>
       </c>
       <c r="C5">
-        <v>0.91591292499762</v>
+        <v>0.95110802073391498</v>
       </c>
       <c r="D5">
-        <v>0.91386219548071701</v>
+        <v>0.94789792272638795</v>
       </c>
       <c r="E5">
-        <v>0.95526597853435102</v>
+        <v>0.97326342038858005</v>
       </c>
       <c r="F5">
-        <v>8.0658901705544905E-2</v>
+        <v>4.6260289344101597E-2</v>
       </c>
       <c r="G5">
         <v>4.6631661327243403</v>
       </c>
       <c r="H5">
-        <v>4.5122819894479802</v>
+        <v>4.7080981270536402</v>
       </c>
       <c r="I5">
-        <v>21.063670690152598</v>
+        <v>21.953192834566</v>
       </c>
       <c r="J5">
-        <v>9.1754481221723196</v>
+        <v>9.3712642597779592</v>
       </c>
       <c r="K5" t="s">
         <v>27</v>
@@ -3105,28 +3244,28 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.89033862681064602</v>
+        <v>0.944000338299258</v>
       </c>
       <c r="D6">
-        <v>0.89169042196672099</v>
+        <v>0.94416856976965102</v>
       </c>
       <c r="E6">
-        <v>0.94375385638417997</v>
+        <v>0.97121055574441095</v>
       </c>
       <c r="F6">
-        <v>0.109507332018559</v>
+        <v>5.60143006007644E-2</v>
       </c>
       <c r="G6">
         <v>4.6785835847737696</v>
       </c>
       <c r="H6">
-        <v>4.3862891773013901</v>
+        <v>4.67291425137517</v>
       </c>
       <c r="I6">
-        <v>20.552632003767499</v>
+        <v>21.8668215042313</v>
       </c>
       <c r="J6">
-        <v>9.0648727620751597</v>
+        <v>9.35149783614896</v>
       </c>
       <c r="K6" t="s">
         <v>27</v>
@@ -3137,31 +3276,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.93748602839737105</v>
+        <v>0.95901469088041702</v>
       </c>
       <c r="C7">
-        <v>0.95982525786682305</v>
+        <v>0.95838637067937404</v>
       </c>
       <c r="D7">
-        <v>0.90042598168243204</v>
+        <v>0.91943391250694795</v>
       </c>
       <c r="E7">
-        <v>0.94894398731637797</v>
+        <v>0.95869167126113297</v>
       </c>
       <c r="F7">
-        <v>4.5231716332018397E-2</v>
+        <v>3.5632998459510103E-2</v>
       </c>
       <c r="G7">
-        <v>4.3861067434146799</v>
+        <v>4.4868303903099997</v>
       </c>
       <c r="H7">
-        <v>4.7286178695436503</v>
+        <v>4.74412682726354</v>
       </c>
       <c r="I7">
-        <v>20.753978502239399</v>
+        <v>21.2939700530716</v>
       </c>
       <c r="J7">
-        <v>9.1147246129583301</v>
+        <v>9.2309572175735592</v>
       </c>
       <c r="K7" t="s">
         <v>27</v>
@@ -3172,31 +3311,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.95501058898561197</v>
+        <v>0.97322972640178496</v>
       </c>
       <c r="C8">
-        <v>0.99773374242231705</v>
+        <v>0.99824132605718996</v>
       </c>
       <c r="D8">
-        <v>0.95288804244967495</v>
+        <v>0.971580206412332</v>
       </c>
       <c r="E8">
-        <v>0.97692361591599997</v>
+        <v>0.986088197902387</v>
       </c>
       <c r="F8">
-        <v>4.3222117792861003E-2</v>
+        <v>2.5415490845142299E-2</v>
       </c>
       <c r="G8">
-        <v>4.46809686491319</v>
+        <v>4.5533366221572802</v>
       </c>
       <c r="H8">
-        <v>4.9153755486182797</v>
+        <v>4.9414136092878502</v>
       </c>
       <c r="I8">
-        <v>21.963180039618599</v>
+        <v>22.501671450306599</v>
       </c>
       <c r="J8">
-        <v>9.3834724135315497</v>
+        <v>9.4947502314451206</v>
       </c>
       <c r="K8" t="s">
         <v>27</v>
@@ -3207,31 +3346,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.95259848705990202</v>
+        <v>0.97184506146743599</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.95260358085937102</v>
+        <v>0.97189913968408503</v>
       </c>
       <c r="E9">
-        <v>0.97691107978872205</v>
+        <v>0.98631952450498706</v>
       </c>
       <c r="F9">
-        <v>4.7759946116156402E-2</v>
+        <v>2.7982666156550699E-2</v>
       </c>
       <c r="G9">
-        <v>4.4568116444387798</v>
+        <v>4.5468583515249996</v>
       </c>
       <c r="H9">
-        <v>4.9265403580364397</v>
+        <v>4.9501192550354798</v>
       </c>
       <c r="I9">
-        <v>21.956623465452601</v>
+        <v>22.509057903476702</v>
       </c>
       <c r="J9">
-        <v>9.3833520024752204</v>
+        <v>9.4969776065605096</v>
       </c>
       <c r="K9" t="s">
         <v>27</v>
@@ -3242,31 +3381,31 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0.97804207187291303</v>
+        <v>0.97781582987516502</v>
       </c>
       <c r="C10">
-        <v>0.877823373948869</v>
+        <v>0.92319611447642302</v>
       </c>
       <c r="D10">
-        <v>0.86040708496741203</v>
+        <v>0.90338448556020401</v>
       </c>
       <c r="E10">
-        <v>0.92663914746585796</v>
+        <v>0.94973581646131</v>
       </c>
       <c r="F10">
-        <v>0.104903012261753</v>
+        <v>5.9628081380639401E-2</v>
       </c>
       <c r="G10">
-        <v>4.5758515826827404</v>
+        <v>4.5747930905858896</v>
       </c>
       <c r="H10">
-        <v>4.3246322789868303</v>
+        <v>4.5699308624436803</v>
       </c>
       <c r="I10">
-        <v>19.8315802829487</v>
+        <v>20.922267408515999</v>
       </c>
       <c r="J10">
-        <v>8.9004838616695707</v>
+        <v>9.1447239530295708</v>
       </c>
       <c r="K10" t="s">
         <v>27</v>
@@ -3277,31 +3416,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>0.99650135139021201</v>
+        <v>0.99669855590412104</v>
       </c>
       <c r="C11">
-        <v>0.91717017533001899</v>
+        <v>0.95182993538673299</v>
       </c>
       <c r="D11">
-        <v>0.91492138156367198</v>
+        <v>0.94861318128531202</v>
       </c>
       <c r="E11">
-        <v>0.95581179414576001</v>
+        <v>0.97363158353358303</v>
       </c>
       <c r="F11">
-        <v>7.9197571790708396E-2</v>
+        <v>4.5535835314306501E-2</v>
       </c>
       <c r="G11">
-        <v>4.6622148648191102</v>
+        <v>4.6631375026207396</v>
       </c>
       <c r="H11">
-        <v>4.5184758839507104</v>
+        <v>4.7116716906770497</v>
       </c>
       <c r="I11">
-        <v>21.088083940816901</v>
+        <v>21.969758129936</v>
       </c>
       <c r="J11">
-        <v>9.1806907487698304</v>
+        <v>9.3748091932977804</v>
       </c>
       <c r="K11" t="s">
         <v>27</v>
@@ -3312,33 +3451,103 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>0.99999231369169395</v>
+        <v>0.999993307635895</v>
       </c>
       <c r="C12">
-        <v>0.89134403879117297</v>
+        <v>0.94488353053645002</v>
       </c>
       <c r="D12">
-        <v>0.89268299298064202</v>
+        <v>0.94503982601356196</v>
       </c>
       <c r="E12">
-        <v>0.94426579581275305</v>
+        <v>0.97166135334265402</v>
       </c>
       <c r="F12">
-        <v>0.108495591544937</v>
+        <v>5.5124972763770201E-2</v>
       </c>
       <c r="G12">
-        <v>4.6785476237378996</v>
+        <v>4.67855227398893</v>
       </c>
       <c r="H12">
-        <v>4.3912423799999196</v>
+        <v>4.6772861582744003</v>
       </c>
       <c r="I12">
-        <v>20.575509839262899</v>
+        <v>21.8869996857341</v>
       </c>
       <c r="J12">
-        <v>9.0697900037378503</v>
+        <v>9.3558384322633206</v>
       </c>
       <c r="K12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>0.99555757929425504</v>
+      </c>
+      <c r="C13">
+        <v>0.95191862357264001</v>
+      </c>
+      <c r="D13">
+        <v>0.94762096601494195</v>
+      </c>
+      <c r="E13">
+        <v>0.97312277799432401</v>
+      </c>
+      <c r="F13">
+        <v>4.4509003438409002E-2</v>
+      </c>
+      <c r="G13">
+        <v>4.6577993481832101</v>
+      </c>
+      <c r="H13">
+        <v>4.7121107077737898</v>
+      </c>
+      <c r="I13">
+        <v>21.946778553083298</v>
+      </c>
+      <c r="J13">
+        <v>9.3699100559570194</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>0.99555172408908998</v>
+      </c>
+      <c r="C14">
+        <v>0.95103652609863898</v>
+      </c>
+      <c r="D14">
+        <v>0.946736047670521</v>
+      </c>
+      <c r="E14">
+        <v>0.97266644635435695</v>
+      </c>
+      <c r="F14">
+        <v>4.5365352719056701E-2</v>
+      </c>
+      <c r="G14">
+        <v>4.6577719541164297</v>
+      </c>
+      <c r="H14">
+        <v>4.7077442200829402</v>
+      </c>
+      <c r="I14">
+        <v>21.926283959106399</v>
+      </c>
+      <c r="J14">
+        <v>9.3655161741993407</v>
+      </c>
+      <c r="K14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4253,24 +4462,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J30"/>
+  <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:J14"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" dimension="1" start="10" max="12" activeRow="13" activeCol="6" previousRow="13" previousCol="6" click="1" r:id="rId2">
-        <pivotArea dataOnly="0" fieldPosition="0">
-          <references count="1">
-            <reference field="0" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="7.54296875" customWidth="1"/>
     <col min="5" max="5" width="19.1796875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -4326,13 +4527,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="4">
-        <v>0.99136900292696495</v>
+        <v>0.99136899635387199</v>
       </c>
       <c r="D5" s="4">
-        <v>4.5813888621856497E-3</v>
+        <v>4.5813906131894396E-3</v>
       </c>
       <c r="E5" s="4">
-        <v>23.623375771724799</v>
+        <v>23.623375615094201</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>20</v>
@@ -4352,13 +4553,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>0.99091917507803795</v>
+        <v>0.99092615927959304</v>
       </c>
       <c r="D6" s="4">
-        <v>8.5736883252808404E-17</v>
+        <v>8.82519515933832E-17</v>
       </c>
       <c r="E6" s="4">
-        <v>23.612656804038199</v>
+        <v>23.612823230885699</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>10</v>
@@ -4407,7 +4608,7 @@
         <v>0.98722503343323798</v>
       </c>
       <c r="D8" s="4">
-        <v>9.9207785631803304E-3</v>
+        <v>9.9207785631803408E-3</v>
       </c>
       <c r="E8" s="4">
         <v>23.524628939568501</v>
@@ -4479,16 +4680,16 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4">
-        <v>0.97573105038694496</v>
+        <v>0.97662121512356104</v>
       </c>
       <c r="D11" s="4">
-        <v>2.21694835358664E-2</v>
+        <v>2.1308152441336499E-2</v>
       </c>
       <c r="E11" s="4">
-        <v>23.250738309727701</v>
+        <v>23.2719500845661</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>18</v>
@@ -4505,16 +4706,16 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4">
-        <v>0.97532377895089495</v>
+        <v>0.97614797485860205</v>
       </c>
       <c r="D12" s="4">
-        <v>2.2502491239377899E-2</v>
+        <v>2.1711299529722599E-2</v>
       </c>
       <c r="E12" s="4">
-        <v>23.241033420683799</v>
+        <v>23.260673221383499</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>12</v>
@@ -4531,16 +4732,16 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4">
-        <v>0.92725626760020197</v>
+        <v>0.97573105038694496</v>
       </c>
       <c r="D13" s="4">
-        <v>2.6002825520783202E-2</v>
+        <v>2.21694835358664E-2</v>
       </c>
       <c r="E13" s="4">
-        <v>22.095630568974201</v>
+        <v>23.250738309727701</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>16</v>
@@ -4557,16 +4758,16 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4">
-        <v>0.92712783124393205</v>
+        <v>0.97532377895089495</v>
       </c>
       <c r="D14" s="4">
-        <v>2.6068282698403999E-2</v>
+        <v>2.2502491239377899E-2</v>
       </c>
       <c r="E14" s="4">
-        <v>22.092570053366</v>
+        <v>23.241033420683799</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>11</v>
@@ -4583,16 +4784,16 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4">
-        <v>0.92526729521434004</v>
+        <v>0.92725626760020197</v>
       </c>
       <c r="D15" s="4">
-        <v>2.0552383596122301E-2</v>
+        <v>2.6002825520783202E-2</v>
       </c>
       <c r="E15" s="4">
-        <v>22.048235258114101</v>
+        <v>22.095630568974201</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>15</v>
@@ -4607,338 +4808,412 @@
         <v>108.852297510215</v>
       </c>
     </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.92712783124393205</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.6068282698403999E-2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>22.092570053366</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.92526729521434004</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.0552383596122398E-2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>22.048235258114101</v>
+      </c>
+    </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E21" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H21" t="s">
         <v>22</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="G19" s="3" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="G22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.96194260005420096</v>
-      </c>
-      <c r="D20" s="4">
-        <v>3.1134989869910399E-2</v>
-      </c>
-      <c r="E20" s="4">
-        <v>22.171879141704</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.99731439143870804</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1.86336682603696E-3</v>
-      </c>
-      <c r="J20" s="4">
-        <v>109.715900988241</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.95773497922703299</v>
-      </c>
-      <c r="D21" s="4">
-        <v>8.5197940036970901E-17</v>
-      </c>
-      <c r="E21" s="4">
-        <v>22.074897408647601</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0.99730319714565996</v>
-      </c>
-      <c r="I21" s="4">
-        <v>2.0956732694438901E-3</v>
-      </c>
-      <c r="J21" s="4">
-        <v>109.714669488968</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.95288804244967495</v>
-      </c>
-      <c r="D22" s="4">
-        <v>4.3222117792861003E-2</v>
-      </c>
-      <c r="E22" s="4">
-        <v>21.963180039618599</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0.99728196184946305</v>
-      </c>
-      <c r="I22" s="4">
-        <v>6.4276069846719505E-17</v>
-      </c>
-      <c r="J22" s="4">
-        <v>109.7123333654</v>
-      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4">
-        <v>0.95260358085937102</v>
+        <v>0.97612421834477203</v>
       </c>
       <c r="D23" s="4">
-        <v>4.7759946116156402E-2</v>
+        <v>1.4231195644233601E-2</v>
       </c>
       <c r="E23" s="4">
-        <v>21.956623465452601</v>
+        <v>22.60691017676</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H23" s="4">
-        <v>0.99572162076090898</v>
+        <v>0.99731439143870804</v>
       </c>
       <c r="I23" s="4">
-        <v>4.6985427305767796E-3</v>
+        <v>1.86336682603696E-3</v>
       </c>
       <c r="J23" s="4">
-        <v>109.540678138272</v>
+        <v>109.715900988241</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4">
-        <v>0.91492138156367198</v>
+        <v>0.97524219908462595</v>
       </c>
       <c r="D24" s="4">
-        <v>7.9197571790708396E-2</v>
+        <v>3.4241887723332303E-10</v>
       </c>
       <c r="E24" s="4">
-        <v>21.088083940816901</v>
+        <v>22.586482725198401</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H24" s="4">
-        <v>0.99299341119529005</v>
+        <v>0.99730319714565996</v>
       </c>
       <c r="I24" s="4">
-        <v>7.4683423372905802E-3</v>
+        <v>2.0956732694438901E-3</v>
       </c>
       <c r="J24" s="4">
-        <v>109.24054412522101</v>
+        <v>109.714669488968</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4">
-        <v>0.91386219548071701</v>
+        <v>0.97189913968408503</v>
       </c>
       <c r="D25" s="4">
-        <v>8.0658901705544905E-2</v>
+        <v>2.7982666156550699E-2</v>
       </c>
       <c r="E25" s="4">
-        <v>21.063670690152598</v>
+        <v>22.509057903476702</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H25" s="4">
-        <v>0.98907383537510196</v>
+        <v>0.99728196184946305</v>
       </c>
       <c r="I25" s="4">
-        <v>4.7045048074090302E-3</v>
+        <v>6.4276069846719505E-17</v>
       </c>
       <c r="J25" s="4">
-        <v>108.809346304057</v>
+        <v>109.7123333654</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" s="4">
-        <v>0.90042598168243204</v>
+        <v>0.971580206412332</v>
       </c>
       <c r="D26" s="4">
-        <v>4.5231716332018397E-2</v>
+        <v>2.5415490845142299E-2</v>
       </c>
       <c r="E26" s="4">
-        <v>20.753978502239399</v>
+        <v>22.501671450306599</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H26" s="4">
-        <v>0.98648977945859895</v>
+        <v>0.99572162076090898</v>
       </c>
       <c r="I26" s="4">
-        <v>5.6750732033414601E-3</v>
+        <v>4.6985427305767796E-3</v>
       </c>
       <c r="J26" s="4">
-        <v>108.525070828322</v>
+        <v>109.540678138272</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4">
-        <v>0.89268299298064202</v>
+        <v>0.94861318128531202</v>
       </c>
       <c r="D27" s="4">
-        <v>0.108495591544937</v>
+        <v>4.5535835314306501E-2</v>
       </c>
       <c r="E27" s="4">
-        <v>20.575509839262899</v>
+        <v>21.969758129936</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H27" s="4">
-        <v>0.98309313032337098</v>
+        <v>0.99299341119529005</v>
       </c>
       <c r="I27" s="4">
-        <v>9.4792263486043297E-3</v>
+        <v>7.4683423372905802E-3</v>
       </c>
       <c r="J27" s="4">
-        <v>108.151400876889</v>
+        <v>109.24054412522101</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4">
-        <v>0.89169042196672099</v>
+        <v>0.94789792272638795</v>
       </c>
       <c r="D28" s="4">
-        <v>0.109507332018559</v>
+        <v>4.6260289344101597E-2</v>
       </c>
       <c r="E28" s="4">
-        <v>20.552632003767499</v>
+        <v>21.953192834566</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H28" s="4">
-        <v>0.980883103586775</v>
+        <v>0.98907383537510196</v>
       </c>
       <c r="I28" s="4">
-        <v>1.13500475601631E-2</v>
+        <v>4.7045048074090302E-3</v>
       </c>
       <c r="J28" s="4">
-        <v>107.90827285557999</v>
+        <v>108.809346304057</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4">
-        <v>0.86040708496741203</v>
+        <v>0.94762096601494195</v>
       </c>
       <c r="D29" s="4">
-        <v>0.104903012261753</v>
+        <v>4.4509003438409002E-2</v>
       </c>
       <c r="E29" s="4">
-        <v>19.8315802829487</v>
+        <v>21.946778553083298</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H29" s="4">
-        <v>0.97018378744825495</v>
+        <v>0.98648977945859895</v>
       </c>
       <c r="I29" s="4">
-        <v>2.0741328529875501E-2</v>
+        <v>5.6750732033414601E-3</v>
       </c>
       <c r="J29" s="4">
-        <v>106.731226660145</v>
+        <v>108.525070828322</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.946736047670521</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4.5365352719056701E-2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>21.926283959106399</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.98309313032337098</v>
+      </c>
+      <c r="I30" s="4">
+        <v>9.4792263486043297E-3</v>
+      </c>
+      <c r="J30" s="4">
+        <v>108.151400876889</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.94503982601356196</v>
+      </c>
+      <c r="D31" s="4">
+        <v>5.5124972763770201E-2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>21.8869996857341</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.980883103586775</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.13500475601631E-2</v>
+      </c>
+      <c r="J31" s="4">
+        <v>107.90827285557999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.94416856976965102</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5.60143006007644E-2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>21.8668215042313</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.97018378744825495</v>
+      </c>
+      <c r="I32" s="4">
+        <v>2.0741328529875501E-2</v>
+      </c>
+      <c r="J32" s="4">
+        <v>106.731226660145</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.91943391250694795</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3.5632998459510103E-2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>21.2939700530716</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.96602712254814804</v>
+      </c>
+      <c r="I33" s="4">
+        <v>2.29539660843152E-2</v>
+      </c>
+      <c r="J33" s="4">
+        <v>106.27394634960601</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.90338448556020401</v>
+      </c>
+      <c r="D34" s="4">
+        <v>5.9628081380639401E-2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>20.922267408515999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="4">
-        <v>0.859362946887402</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0.10542656968555</v>
-      </c>
-      <c r="E30" s="4">
-        <v>19.807513874707801</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="4">
-        <v>0.96602712254814804</v>
-      </c>
-      <c r="I30" s="4">
-        <v>2.29539660843152E-2</v>
-      </c>
-      <c r="J30" s="4">
-        <v>106.27394634960601</v>
+      <c r="C35" s="4">
+        <v>0.90318756362812402</v>
+      </c>
+      <c r="D35" s="4">
+        <v>5.97486322518632E-2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>20.917706722133399</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="B18:E30">
     <sortCondition descending="1" ref="C18"/>
   </sortState>
-  <conditionalFormatting pivot="1" sqref="C4:C15">
-    <cfRule type="colorScale" priority="19">
+  <conditionalFormatting pivot="1" sqref="C4:C17">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4947,8 +5222,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="D4:D15">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting pivot="1" sqref="D4:D17">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4957,8 +5232,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="D4:D15">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting pivot="1" sqref="D4:D17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4967,8 +5242,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="E4:E15">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting pivot="1" sqref="E4:E17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4977,7 +5252,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="C20:C30">
+  <conditionalFormatting pivot="1" sqref="C23:C28 C31:C35">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="9" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="D23:D28 D31:D35">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <color theme="9" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E23:E28 E31:E35">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4987,17 +5282,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="D20:D30">
+  <conditionalFormatting pivot="1" sqref="H4:H15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color theme="9" tint="0.79998168889431442"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <color theme="9" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="E20:E30">
+  <conditionalFormatting pivot="1" sqref="I4:I15">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -5007,28 +5302,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="H4:H15">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color theme="9" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="I4:I15">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color theme="9" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="I4:I15">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5038,6 +5313,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="J4:J15">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="9" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="H23:H33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="9" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="J23:J33">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="9" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="I23:I33">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5047,17 +5352,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="H20:H30">
+  <conditionalFormatting pivot="1" sqref="I23:I33">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color theme="9" tint="0.79998168889431442"/>
         <color theme="9" tint="-0.249977111117893"/>
+        <color theme="9" tint="0.59999389629810485"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="J20:J30">
+  <conditionalFormatting pivot="1" sqref="C23:C35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5067,8 +5372,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="I20:I30">
+  <conditionalFormatting pivot="1" sqref="D23:D35">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <color theme="9" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E23:E35">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5077,16 +5392,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="I20:I30">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <color theme="9" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>